<commit_message>
0.0.1: Enable TestCaseDataList export.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoRestAutotestTestCaseData.xlsx
+++ b/meta/program/BlancoRestAutotestTestCaseData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestAutotest/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{583AABE6-C5ED-1941-9F68-D74233A5DD9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9127B3E3-818D-6244-BAA4-F64D7962A18B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10240" yWindow="2900" windowWidth="23360" windowHeight="17540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="48">
   <si>
     <t>バリューオブジェクト定義書</t>
   </si>
@@ -282,6 +282,30 @@
     <rPh sb="9" eb="11">
       <t xml:space="preserve">カクノウシマス。 </t>
     </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>simpleExpectId</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>電文クラスの短縮名を格納します。</t>
+    <rPh sb="0" eb="2">
+      <t xml:space="preserve">デンブｎ </t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t xml:space="preserve">タンシュク </t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t xml:space="preserve">セイシキメイヲ </t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t xml:space="preserve">カクノウシマス。 </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>simpleInputId</t>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -1227,10 +1251,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G52"/>
+  <dimension ref="A1:G54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1547,73 +1571,91 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="40">
-        <f>A28+1</f>
+        <f t="shared" ref="A29:A33" si="0">A28+1</f>
         <v>3</v>
       </c>
       <c r="B29" s="41" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="C29" s="42" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="D29" s="42"/>
       <c r="E29" s="42" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="F29" s="43"/>
       <c r="G29"/>
     </row>
-    <row r="30" spans="1:7" ht="26.25" customHeight="1">
+    <row r="30" spans="1:7">
       <c r="A30" s="40">
-        <f>A29+1</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B30" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="D30" s="42"/>
+      <c r="E30" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="F30" s="43"/>
+      <c r="G30"/>
+    </row>
+    <row r="31" spans="1:7" ht="26.25" customHeight="1">
+      <c r="A31" s="40">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B31" s="41" t="s">
         <v>40</v>
-      </c>
-      <c r="C30" s="42" t="s">
-        <v>41</v>
-      </c>
-      <c r="D30" s="42"/>
-      <c r="E30" s="46" t="s">
-        <v>33</v>
-      </c>
-      <c r="F30" s="47"/>
-      <c r="G30"/>
-    </row>
-    <row r="31" spans="1:7">
-      <c r="A31" s="40">
-        <f>A30+1</f>
-        <v>5</v>
-      </c>
-      <c r="B31" s="41" t="s">
-        <v>34</v>
       </c>
       <c r="C31" s="42" t="s">
         <v>41</v>
       </c>
       <c r="D31" s="42"/>
-      <c r="E31" s="42" t="s">
+      <c r="E31" s="46" t="s">
+        <v>33</v>
+      </c>
+      <c r="F31" s="47"/>
+      <c r="G31"/>
+    </row>
+    <row r="32" spans="1:7" ht="26.25" customHeight="1">
+      <c r="A32" s="40">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B32" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="C32" s="42" t="s">
+        <v>41</v>
+      </c>
+      <c r="D32" s="42"/>
+      <c r="E32" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="F32" s="47"/>
+      <c r="G32"/>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="40">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B33" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33" s="42" t="s">
+        <v>41</v>
+      </c>
+      <c r="D33" s="42"/>
+      <c r="E33" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="F31" s="43"/>
-      <c r="G31"/>
-    </row>
-    <row r="32" spans="1:7">
-      <c r="A32" s="40"/>
-      <c r="B32" s="41"/>
-      <c r="C32" s="42"/>
-      <c r="D32" s="42"/>
-      <c r="E32" s="42"/>
-      <c r="F32" s="43"/>
-      <c r="G32"/>
-    </row>
-    <row r="33" spans="1:7">
-      <c r="A33" s="40"/>
-      <c r="B33" s="41"/>
-      <c r="C33" s="42"/>
-      <c r="D33" s="42"/>
-      <c r="E33" s="42"/>
       <c r="F33" s="43"/>
       <c r="G33"/>
     </row>
@@ -1713,7 +1755,7 @@
       <c r="C44" s="42"/>
       <c r="D44" s="42"/>
       <c r="E44" s="42"/>
-      <c r="F44" s="44"/>
+      <c r="F44" s="43"/>
       <c r="G44"/>
     </row>
     <row r="45" spans="1:7">
@@ -1731,7 +1773,8 @@
       <c r="C46" s="42"/>
       <c r="D46" s="42"/>
       <c r="E46" s="42"/>
-      <c r="F46" s="43"/>
+      <c r="F46" s="44"/>
+      <c r="G46"/>
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="40"/>
@@ -1740,6 +1783,7 @@
       <c r="D47" s="42"/>
       <c r="E47" s="42"/>
       <c r="F47" s="43"/>
+      <c r="G47"/>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="40"/>
@@ -1774,16 +1818,32 @@
       <c r="F51" s="43"/>
     </row>
     <row r="52" spans="1:6">
-      <c r="A52" s="45"/>
-      <c r="B52" s="23"/>
-      <c r="C52" s="24"/>
-      <c r="D52" s="24"/>
-      <c r="E52" s="24"/>
-      <c r="F52" s="25"/>
+      <c r="A52" s="40"/>
+      <c r="B52" s="41"/>
+      <c r="C52" s="42"/>
+      <c r="D52" s="42"/>
+      <c r="E52" s="42"/>
+      <c r="F52" s="43"/>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" s="40"/>
+      <c r="B53" s="41"/>
+      <c r="C53" s="42"/>
+      <c r="D53" s="42"/>
+      <c r="E53" s="42"/>
+      <c r="F53" s="43"/>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54" s="45"/>
+      <c r="B54" s="23"/>
+      <c r="C54" s="24"/>
+      <c r="D54" s="24"/>
+      <c r="E54" s="24"/>
+      <c r="F54" s="25"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="E30:F30"/>
+  <mergeCells count="12">
+    <mergeCell ref="E32:F32"/>
     <mergeCell ref="E19:E20"/>
     <mergeCell ref="E25:E26"/>
     <mergeCell ref="A25:A26"/>
@@ -1794,10 +1854,11 @@
     <mergeCell ref="B19:B20"/>
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E31:F31"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D58" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D60" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Some important values are added to testCaseData.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoRestAutotestTestCaseData.xlsx
+++ b/meta/program/BlancoRestAutotestTestCaseData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestAutotest/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9127B3E3-818D-6244-BAA4-F64D7962A18B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DEEA5F6-3532-7F42-B36F-E9B4FFE0F6D5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10240" yWindow="2900" windowWidth="23360" windowHeight="17540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="62">
   <si>
     <t>バリューオブジェクト定義書</t>
   </si>
@@ -306,6 +306,80 @@
   </si>
   <si>
     <t>simpleInputId</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>inputColumnMax</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>java.lang.Integer</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>このテストケースのInputカラムの最大値を保持します。</t>
+    <rPh sb="18" eb="21">
+      <t xml:space="preserve">サイダイチ </t>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t xml:space="preserve">ホジシマス。 </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>expectedColumnMax</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>このテストケースのExpectカラムの最大値を保持します。</t>
+    <rPh sb="19" eb="22">
+      <t xml:space="preserve">サイダイチ </t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t xml:space="preserve">ホジシマス。 </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>propertyMap</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>java.util.Map&lt;String, String&gt;</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Input?/Expected? ごとに入っているはずのプロパティリストを保持する</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>java.util.Map&lt;String, Integer&gt;</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>property.property... という形式で、そのプロパティの横幅（定義書のカラム数）を保持する。</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Expect? のカラムごとの比較方法を保持します。</t>
+    <rPh sb="15" eb="19">
+      <t xml:space="preserve">ヒカクホウホウ </t>
+    </rPh>
+    <rPh sb="20" eb="22">
+      <t xml:space="preserve">ホジシマス。 </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>propertySizeMap</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>assertKindList</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>java.util.List&lt;String&gt;</t>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -1254,7 +1328,7 @@
   <dimension ref="A1:G54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1571,7 +1645,7 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="40">
-        <f t="shared" ref="A29:A33" si="0">A28+1</f>
+        <f t="shared" ref="A29:A38" si="0">A28+1</f>
         <v>3</v>
       </c>
       <c r="B29" s="41" t="s">
@@ -1660,47 +1734,96 @@
       <c r="G33"/>
     </row>
     <row r="34" spans="1:7">
-      <c r="A34" s="40"/>
-      <c r="B34" s="41"/>
-      <c r="C34" s="42"/>
-      <c r="D34" s="42"/>
-      <c r="E34" s="42"/>
+      <c r="A34" s="40">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B34" s="41" t="s">
+        <v>48</v>
+      </c>
+      <c r="C34" s="42" t="s">
+        <v>49</v>
+      </c>
+      <c r="D34" s="42">
+        <v>0</v>
+      </c>
+      <c r="E34" s="42" t="s">
+        <v>50</v>
+      </c>
       <c r="F34" s="43"/>
       <c r="G34"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="40"/>
-      <c r="B35" s="41"/>
-      <c r="C35" s="42"/>
-      <c r="D35" s="42"/>
-      <c r="E35" s="42"/>
+      <c r="A35" s="40">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B35" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="C35" s="42" t="s">
+        <v>49</v>
+      </c>
+      <c r="D35" s="42">
+        <v>0</v>
+      </c>
+      <c r="E35" s="42" t="s">
+        <v>52</v>
+      </c>
       <c r="F35" s="43"/>
       <c r="G35"/>
     </row>
     <row r="36" spans="1:7">
-      <c r="A36" s="40"/>
-      <c r="B36" s="41"/>
-      <c r="C36" s="42"/>
+      <c r="A36" s="40">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B36" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="C36" s="42" t="s">
+        <v>54</v>
+      </c>
       <c r="D36" s="42"/>
-      <c r="E36" s="42"/>
+      <c r="E36" s="42" t="s">
+        <v>55</v>
+      </c>
       <c r="F36" s="43"/>
       <c r="G36"/>
     </row>
     <row r="37" spans="1:7">
-      <c r="A37" s="40"/>
-      <c r="B37" s="41"/>
-      <c r="C37" s="42"/>
+      <c r="A37" s="40">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B37" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="C37" s="42" t="s">
+        <v>56</v>
+      </c>
       <c r="D37" s="42"/>
-      <c r="E37" s="42"/>
+      <c r="E37" s="42" t="s">
+        <v>57</v>
+      </c>
       <c r="F37" s="43"/>
       <c r="G37"/>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" s="40"/>
-      <c r="B38" s="41"/>
-      <c r="C38" s="42"/>
+      <c r="A38" s="40">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B38" s="41" t="s">
+        <v>60</v>
+      </c>
+      <c r="C38" s="42" t="s">
+        <v>61</v>
+      </c>
       <c r="D38" s="42"/>
-      <c r="E38" s="42"/>
+      <c r="E38" s="42" t="s">
+        <v>58</v>
+      </c>
       <c r="F38" s="43"/>
       <c r="G38"/>
     </row>

</xml_diff>

<commit_message>
Add API smiple Id into testCaseData structure.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoRestAutotestTestCaseData.xlsx
+++ b/meta/program/BlancoRestAutotestTestCaseData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestAutotest/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DEEA5F6-3532-7F42-B36F-E9B4FFE0F6D5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B42E4D5-207C-9941-B487-38F64C88189E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10240" yWindow="2900" windowWidth="23360" windowHeight="17540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="64">
   <si>
     <t>バリューオブジェクト定義書</t>
   </si>
@@ -380,6 +380,29 @@
   </si>
   <si>
     <t>java.util.List&lt;String&gt;</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>targetApiSimpleId</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>対象APIの電文処理IDの短縮名を格納します。</t>
+    <rPh sb="0" eb="2">
+      <t xml:space="preserve">タイショウ </t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t xml:space="preserve">デンブｎ </t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t xml:space="preserve">ショリ </t>
+    </rPh>
+    <rPh sb="13" eb="16">
+      <t xml:space="preserve">タンシュクメイ </t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t xml:space="preserve">カクノウシマス。 </t>
+    </rPh>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -1327,8 +1350,8 @@
   </sheetPr>
   <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1645,7 +1668,7 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="40">
-        <f t="shared" ref="A29:A38" si="0">A28+1</f>
+        <f t="shared" ref="A29:A39" si="0">A28+1</f>
         <v>3</v>
       </c>
       <c r="B29" s="41" t="s">
@@ -1828,11 +1851,20 @@
       <c r="G38"/>
     </row>
     <row r="39" spans="1:7">
-      <c r="A39" s="40"/>
-      <c r="B39" s="41"/>
-      <c r="C39" s="42"/>
+      <c r="A39" s="40">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B39" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="C39" s="42" t="s">
+        <v>41</v>
+      </c>
       <c r="D39" s="42"/>
-      <c r="E39" s="42"/>
+      <c r="E39" s="42" t="s">
+        <v>63</v>
+      </c>
       <c r="F39" s="43"/>
       <c r="G39"/>
     </row>

</xml_diff>

<commit_message>
0.0.3: HTTP method information is added to TestCaseData.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoRestAutotestTestCaseData.xlsx
+++ b/meta/program/BlancoRestAutotestTestCaseData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestAutotest/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B42E4D5-207C-9941-B487-38F64C88189E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CC679F8-CA4C-E14F-86D9-B27FA67DADBD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10240" yWindow="2900" windowWidth="23360" windowHeight="17540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="66">
   <si>
     <t>バリューオブジェクト定義書</t>
   </si>
@@ -402,6 +402,17 @@
     </rPh>
     <rPh sb="17" eb="19">
       <t xml:space="preserve">カクノウシマス。 </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>method</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>このテストケースが対象とするHTTPメソッド</t>
+    <rPh sb="9" eb="11">
+      <t xml:space="preserve">タイショウ </t>
     </rPh>
     <phoneticPr fontId="3"/>
   </si>
@@ -1350,8 +1361,8 @@
   </sheetPr>
   <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1668,7 +1679,7 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="40">
-        <f t="shared" ref="A29:A39" si="0">A28+1</f>
+        <f t="shared" ref="A29:A40" si="0">A28+1</f>
         <v>3</v>
       </c>
       <c r="B29" s="41" t="s">
@@ -1869,11 +1880,20 @@
       <c r="G39"/>
     </row>
     <row r="40" spans="1:7">
-      <c r="A40" s="40"/>
-      <c r="B40" s="41"/>
-      <c r="C40" s="42"/>
+      <c r="A40" s="40">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B40" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="C40" s="42" t="s">
+        <v>41</v>
+      </c>
       <c r="D40" s="42"/>
-      <c r="E40" s="42"/>
+      <c r="E40" s="42" t="s">
+        <v>65</v>
+      </c>
       <c r="F40" s="43"/>
       <c r="G40"/>
     </row>

</xml_diff>